<commit_message>
code for mac, UI start
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -468,9 +468,9 @@
 ③ ✨인스타그램 게시물✨에 좋아요 누르고 댓글로 비바샘 계정 아이디를 남겨 참여 인증하기
 (비바샘 계정 아이디를 남겨주시면, 당첨 확률 UP!)
 🎁 상품
-◽1등 : 교촌치킨 콤보웨지감자세트(40명)
-◽2등 : 신세계 모바일 상품권 10,000원권 (50명)
-◽3등 : 스타벅스 아이스 카페 라떼 (100명)
+◽1등 : 교촌치킨 콤보웨지감자세트
+◽2등 : 신세계 모바일 상품권 10,000원권
+◽3등 : 스타벅스 아이스 카페 라떼
 ❗❗ 게시물에 해시태그를 추가하지 않으면 참여로 인정되지 않으니 상단의 해시태그를 꼭 추가해주세요
 🔎 비바샘은 초/중/고 학교 선생님을 위한 수업지원 사이트입니다. 회원가입 및 사이트 자료 이용을 위해서는 선생님 인증이 필요합니다
 #비상교육 #비바샘 #초등비바샘 #중고등비바샘 #visang</t>

</xml_diff>